<commit_message>
Added more condition in Consumer
</commit_message>
<xml_diff>
--- a/C#Models/CSharpLoansProducer/Loan Quotes.xlsx
+++ b/C#Models/CSharpLoansProducer/Loan Quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/horea_soanca_uipath_com/Documents/Documents/Work/Demo_REF/Loans_Producer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\C#Models\CSharpLoansProducer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{050CBA71-0116-4F12-AE4B-BEE448199A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C848346E-A016-4F28-A48F-220E9B06FC7C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ABBD42-A525-4554-9641-02434DB4A503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AB1519B2-5C0E-448B-8AC7-B3DEE8C41096}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB1519B2-5C0E-448B-8AC7-B3DEE8C41096}"/>
   </bookViews>
   <sheets>
     <sheet name="Loan Quotes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>LoanEmail</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD367E9C-F7F3-473F-AC86-C94BB6C9B28F}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,6 +642,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7">
+        <v>100000</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7">
+        <v>252000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>